<commit_message>
Autofill fields from selected record in datagrid
</commit_message>
<xml_diff>
--- a/Iteration Plan.xlsx
+++ b/Iteration Plan.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="137">
   <si>
     <t xml:space="preserve">User Story </t>
   </si>
@@ -61,14 +61,6 @@
   </si>
   <si>
     <t>Technicians can be assigned Wos</t>
-  </si>
-  <si>
-    <t>-Connect WO queue to the message box and 'new request'list
--Add functionality to each list item to prompt to 'Proceed' window.
--Code to add functionality to 'accept' button and link it to the 'active Technician WOs' table
--DB connection to status table and RMA request to record above
-- Code to track dates for ' Assigned' Status
--Code to send out email notifications</t>
   </si>
   <si>
     <t>Technicians can delegate requests</t>
@@ -671,65 +663,6 @@
   </si>
   <si>
     <r>
-      <t>-Code to add functionality to ' delegate' button</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(both on Prceed Window &amp; update screen) and further link it to 'update message' prompt window
--</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Create DB for various information sections like resolution,description etc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-DB connection to the Status update section with the prompt window.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
--Add functionality to automatically record the dates when user enters information in status update section.
--Code to send notification to Supervisor, asking for approval/putting the request on 'hold'</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF00B0F0"/>
@@ -910,54 +843,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>-DB connection</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>-Business logic to categorize WO on the basis of number of pieces.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-Code to assign categories to each request, if quantity provided.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Link the radio buttons to the 'Category' table
--Enable radio buttons to choose the desired category and link it to the request.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-Add functionality to 'Update' button to reflect the changes in the DB.</t>
     </r>
   </si>
   <si>
@@ -1464,36 +1349,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">-Worked on Delegate button(only on Update Panel) 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Refer designed Wireframe to work with Proceed Window and Delegate Button. 
--To reach to Proceed window, automated request assignment is needed --&gt; how ?
- </t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Done!</t>
     </r>
     <r>
@@ -1669,6 +1524,194 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> Completed/Near completion </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">-Connect WO queue to the message box and 'new request'list
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-Add functionality to each list item to prompt to 'Proceed' window.
+-Code to add functionality to 'accept' button and link it to the 'active Technician WOs' table
+-DB connection to status table and RMA request to record above</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Code to track dates for ' Assigned' Status
+-Code to send out email notifications</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>-Code to add functionality to ' delegate' button(both on Prceed Window &amp; update screen) and further link it to 'update message' prompt window</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Create DB for various information sections like resolution,description etc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-DB connection to the Status update section with the prompt window.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+-Add functionality to automatically record the dates when user enters information in status update section.
+-Code to send notification to Supervisor, asking for approval/putting the request on 'hold'</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">-To reach to Proceed window, automated request assignment is needed --&gt; how ?
+ </t>
+  </si>
+  <si>
+    <r>
+      <t>-Business logic to categorize WO on the basis of number of pieces.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-Code to assign categories to each request, if quantity provided.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Link the radio buttons to the 'Category' table
+-Enable radio buttons to choose the desired category and link it to the request.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-Add functionality to 'Update' button to reflect the changes in the DB.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">After the request is acceptd by theTech, what would be the chnge in status ?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Suggestion:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Until the request is accepted by the tech, the status remains 'waiting  to be assigned'.Once accpeted it is changed to 'assigned' and added in Tech WO queue</t>
     </r>
   </si>
 </sst>
@@ -1676,7 +1719,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1777,6 +1820,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1904,7 +1955,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1942,6 +1993,33 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1983,30 +2061,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2313,7 +2367,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2328,15 +2382,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="108.75" customHeight="1">
-      <c r="A1" s="35" t="s">
-        <v>135</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
+      <c r="A1" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:7" ht="15.75">
       <c r="A2" s="5"/>
@@ -2346,15 +2400,15 @@
       <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="15"/>
+      <c r="D2" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="24"/>
       <c r="F2" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="109.5" customHeight="1">
@@ -2365,19 +2419,19 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="G3" s="28" t="s">
-        <v>100</v>
+        <v>96</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="150">
@@ -2385,74 +2439,74 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="1"/>
+      <c r="G4" s="15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="65.25" customHeight="1">
+      <c r="A5" s="25">
+        <v>3</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="29" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="65.25" customHeight="1">
-      <c r="A5" s="16">
-        <v>3</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="G5" s="34" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="67.5" customHeight="1">
+      <c r="A6" s="26"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="25" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="67.5" customHeight="1">
-      <c r="A6" s="17"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="4" t="s">
+      <c r="G6" s="35"/>
+    </row>
+    <row r="7" spans="1:7" ht="46.5" customHeight="1">
+      <c r="A7" s="27"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="26"/>
-    </row>
-    <row r="7" spans="1:7" ht="46.5" customHeight="1">
-      <c r="A7" s="18"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="27"/>
+      <c r="G7" s="36"/>
     </row>
     <row r="8" spans="1:7" ht="90">
       <c r="A8" s="6">
@@ -2462,17 +2516,17 @@
         <v>9</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="13" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="150">
@@ -2483,36 +2537,38 @@
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>11</v>
+        <v>132</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="7"/>
+      <c r="F9" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" ht="165">
       <c r="A10" s="6">
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>58</v>
-      </c>
       <c r="F10" s="4"/>
-      <c r="G10" s="9" t="s">
-        <v>131</v>
+      <c r="G10" s="12" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="75">
@@ -2520,16 +2576,16 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>126</v>
+        <v>17</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>123</v>
       </c>
       <c r="D11" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="7"/>
@@ -2539,16 +2595,16 @@
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="7"/>
@@ -2558,14 +2614,14 @@
         <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="17" t="s">
         <v>14</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>15</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="12"/>
@@ -2575,20 +2631,20 @@
         <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="32" t="s">
-        <v>132</v>
+      <c r="G14" s="18" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="180">
@@ -2596,16 +2652,16 @@
         <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="7"/>
@@ -2615,16 +2671,16 @@
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="7"/>
@@ -2634,20 +2690,20 @@
         <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D17" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="F17" s="4"/>
-      <c r="G17" s="29" t="s">
-        <v>128</v>
+      <c r="G17" s="15" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="60">
@@ -2655,35 +2711,35 @@
         <v>14</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>31</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="G18" s="33"/>
+        <v>109</v>
+      </c>
+      <c r="G18" s="19"/>
     </row>
     <row r="19" spans="1:7" ht="114" customHeight="1">
       <c r="A19" s="6">
         <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="7"/>
@@ -2693,20 +2749,20 @@
         <v>16</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>76</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="9" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="135">
@@ -2714,20 +2770,20 @@
         <v>17</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="120">
@@ -2735,20 +2791,20 @@
         <v>18</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D22" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="105">
@@ -2756,15 +2812,15 @@
         <v>19</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="1"/>
       <c r="E23" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G23" s="7"/>
     </row>
@@ -2773,20 +2829,20 @@
         <v>20</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="31" t="s">
-        <v>34</v>
-      </c>
       <c r="D24" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="10" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="194.25" customHeight="1">
@@ -2794,22 +2850,22 @@
         <v>21</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G25" s="30" t="s">
-        <v>124</v>
+      <c r="G25" s="16" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="120">
@@ -2817,20 +2873,20 @@
         <v>22</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D26" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="66" customHeight="1">
@@ -2838,16 +2894,16 @@
         <v>23</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="D27" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="7"/>
@@ -2864,7 +2920,7 @@
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="7"/>
@@ -2881,11 +2937,11 @@
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F29" s="4"/>
-      <c r="G29" s="34" t="s">
-        <v>134</v>
+      <c r="G29" s="20" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="135">
@@ -2896,15 +2952,15 @@
         <v>5</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="120">
@@ -2912,14 +2968,14 @@
         <v>27</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="7"/>
@@ -2959,10 +3015,10 @@
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="15"/>
+      <c r="C1" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:4" ht="60">
       <c r="A2" s="6">
@@ -2972,10 +3028,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45">
@@ -2983,13 +3039,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="90">
@@ -2997,13 +3053,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="75">
@@ -3011,13 +3067,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="60">
@@ -3025,13 +3081,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="45">
@@ -3042,10 +3098,10 @@
         <v>9</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="90">
@@ -3056,10 +3112,10 @@
         <v>10</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="135">
@@ -3067,13 +3123,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="60">
@@ -3081,13 +3137,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="75">
@@ -3095,13 +3151,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="60">
@@ -3109,11 +3165,11 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="45">
@@ -3121,13 +3177,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="60">
@@ -3135,13 +3191,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="60">
@@ -3149,13 +3205,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="60">
@@ -3163,13 +3219,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="60">
@@ -3177,11 +3233,11 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="90">
@@ -3189,13 +3245,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="75">
@@ -3203,13 +3259,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="90">
@@ -3217,13 +3273,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="90">
@@ -3231,13 +3287,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="105">
@@ -3245,11 +3301,11 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="60">
@@ -3257,13 +3313,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="60">
@@ -3271,13 +3327,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="75">
@@ -3285,13 +3341,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="75">
@@ -3299,13 +3355,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="60">
@@ -3317,7 +3373,7 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="105">
@@ -3329,7 +3385,7 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="45">
@@ -3341,7 +3397,7 @@
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="75">
@@ -3349,11 +3405,11 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -3376,7 +3432,7 @@
   <sheetData>
     <row r="8" spans="6:6">
       <c r="F8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>